<commit_message>
2014 04 14 09:17
Estrutura do trab
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Ação</t>
   </si>
@@ -122,9 +122,6 @@
     <t>notpad++</t>
   </si>
   <si>
-    <t>Atividades estão detalhadas no arquivo "BD2 Trabalho Funçoes NF OK.pdff"</t>
-  </si>
-  <si>
     <t>Obs todas as tabélas e funções serão em aquivos individuais</t>
   </si>
   <si>
@@ -138,6 +135,12 @@
   </si>
   <si>
     <t>T3 - Avalicação 2014-2</t>
+  </si>
+  <si>
+    <t>Atividades estão detalhadas no arquivo "BD2 Trabalho Avaliação 2014 01"</t>
+  </si>
+  <si>
+    <t>Entrega</t>
   </si>
 </sst>
 </file>
@@ -330,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -356,9 +359,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -406,6 +406,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,6 +626,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="5" name="AutoShape 23"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9772650" cy="9582150"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 23"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -945,69 +999,75 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="57" style="19" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="18" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="18" customWidth="1"/>
-    <col min="7" max="7" width="23" style="21" customWidth="1"/>
-    <col min="8" max="8" width="30" style="19" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="57" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="17" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="23" style="20" customWidth="1"/>
+    <col min="8" max="8" width="30" style="18" customWidth="1"/>
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="17" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="26">
+        <v>41757</v>
+      </c>
+      <c r="G2" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1019,7 +1079,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1043,7 +1103,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -1178,7 +1238,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>20</v>
@@ -1190,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>14</v>
@@ -1214,27 +1274,27 @@
         <v>9</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" s="20" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:8" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="21">
         <f>COUNTA(B4:B20)</f>
         <v>5</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:G21"/>

</xml_diff>

<commit_message>
2014 04 22 21:37
Criação da agenda de atividades
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -10,9 +10,9 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$38</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
   <si>
     <t>Ação</t>
   </si>
@@ -110,27 +110,15 @@
     <t>Ativid:</t>
   </si>
   <si>
-    <t>Pasta T1 - Funções</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estrutura da atividade </t>
   </si>
   <si>
-    <t>Tabela tipoUtilitario</t>
-  </si>
-  <si>
-    <t>notpad++</t>
-  </si>
-  <si>
     <t>Obs todas as tabélas e funções serão em aquivos individuais</t>
   </si>
   <si>
     <t xml:space="preserve">Todas as tabelas e funções </t>
   </si>
   <si>
-    <t>?!</t>
-  </si>
-  <si>
     <t>T3 - Avalicação 2014-1</t>
   </si>
   <si>
@@ -141,13 +129,136 @@
   </si>
   <si>
     <t>Entrega</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-5</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-7</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-9</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-10</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-12</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-13</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-14</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-15</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-16</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-17</t>
+  </si>
+  <si>
+    <t>Tabela clientes</t>
+  </si>
+  <si>
+    <t>Tabela funcionarios</t>
+  </si>
+  <si>
+    <t>Insert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tabela Produtos </t>
+  </si>
+  <si>
+    <t>Tabela venda</t>
+  </si>
+  <si>
+    <t>Tabela venda_Intens</t>
+  </si>
+  <si>
+    <t>Tabela Comissoes</t>
+  </si>
+  <si>
+    <t>Comdo</t>
+  </si>
+  <si>
+    <t>Alter</t>
+  </si>
+  <si>
+    <t>item 3</t>
+  </si>
+  <si>
+    <t>item 4</t>
+  </si>
+  <si>
+    <t>item 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item 6 </t>
+  </si>
+  <si>
+    <t>item  7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">item  8 </t>
+  </si>
+  <si>
+    <t>item 9</t>
+  </si>
+  <si>
+    <t>item 10</t>
+  </si>
+  <si>
+    <t>item 20</t>
+  </si>
+  <si>
+    <t>item 11</t>
+  </si>
+  <si>
+    <t>item 12</t>
+  </si>
+  <si>
+    <t>item 13</t>
+  </si>
+  <si>
+    <t>item 14</t>
+  </si>
+  <si>
+    <t>item 15</t>
+  </si>
+  <si>
+    <t>item 16</t>
+  </si>
+  <si>
+    <t>item 17</t>
+  </si>
+  <si>
+    <t>item 18</t>
+  </si>
+  <si>
+    <t>item 19</t>
+  </si>
+  <si>
+    <t>item 21</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Notpad++</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -192,6 +303,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="ArialMT"/>
+    </font>
   </fonts>
   <fills count="22">
     <fill>
@@ -333,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -351,9 +467,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -399,6 +512,12 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -408,11 +527,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,7 +569,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -486,7 +612,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -529,7 +655,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -572,7 +698,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -620,7 +746,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -668,7 +794,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -784,7 +910,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -819,7 +944,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -995,91 +1119,91 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.140625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="57" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" style="17" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="23" style="20" customWidth="1"/>
-    <col min="8" max="8" width="30" style="18" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="57" style="17" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" style="16" customWidth="1"/>
+    <col min="7" max="7" width="23" style="19" customWidth="1"/>
+    <col min="8" max="8" width="30" style="17" customWidth="1"/>
     <col min="9" max="16384" width="9.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="26">
+    <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
+      <c r="A1" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" customHeight="1">
+      <c r="A2" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="22">
         <v>41757</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="23">
         <v>0.5</v>
       </c>
-      <c r="H2" s="9"/>
-    </row>
-    <row r="3" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" ht="33.75" customHeight="1">
+      <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="25.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1095,7 +1219,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -1119,185 +1243,766 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="21" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+    <row r="7" spans="1:8" ht="21" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C7" s="3"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
+    <row r="10" spans="1:8" ht="21" customHeight="1">
+      <c r="A10" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="16">
+        <v>6</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" customHeight="1">
+      <c r="A11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="16">
+        <v>6</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="16">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" customHeight="1">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" ht="21" customHeight="1">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="3">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" ht="21" customHeight="1">
+      <c r="A15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="28"/>
+      <c r="D15" s="3">
+        <v>8</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="3"/>
+    <row r="16" spans="1:8" ht="21" customHeight="1">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3"/>
+    <row r="17" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="3">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="F18" s="4"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="3">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="20.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>20</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="28"/>
       <c r="D19" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="28"/>
+      <c r="D20" s="3">
+        <v>13</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="3">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="3">
+        <v>15</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="3">
+        <v>16</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="3">
+        <v>17</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="3">
+        <v>18</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="3">
+        <v>19</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="3">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" ht="21" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="3">
+        <v>21</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" ht="21" customHeight="1">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="3">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="21" customHeight="1">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="3">
+        <v>23</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="21" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" s="3">
+        <v>24</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="21" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="3">
+        <v>25</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="21" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D33" s="3">
         <v>26</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="21" customHeight="1">
+      <c r="A34" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D34" s="3">
+        <v>27</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" ht="21" customHeight="1">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="3">
+        <v>28</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" ht="21" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="3">
+        <v>29</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G36" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" ht="21" customHeight="1">
+      <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B37" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="3">
-        <v>12</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="C37" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="3">
+        <v>30</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="3" t="s">
+      <c r="F37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" s="19" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A38" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="21">
-        <f>COUNTA(B4:B20)</f>
-        <v>5</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="B38" s="20">
+        <f>COUNTA(B4:B37)</f>
+        <v>34</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G21"/>
+  <autoFilter ref="A3:G38"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 04 23 14:55
Ediação da agenda
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author/>
+    <author>Portaria</author>
   </authors>
   <commentList>
     <comment ref="F3" authorId="0">
@@ -28,17 +28,27 @@
           <rPr>
             <b/>
             <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Estatus da atividade:
-========================
+          <t xml:space="preserve">
+Estatus da atividade:
+====================
 ?  = Em aberto
 !   = Concluida
 ?! = Em execução
 !!  = Revisado ok
-*  =  Dúvida (Aguarda solução)
+*  =  Dúvida (Aguarda solução)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -258,7 +268,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -297,16 +307,22 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="ArialMT"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="ArialMT"/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -518,15 +534,6 @@
     <xf numFmtId="20" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -534,11 +541,20 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1123,7 +1139,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1140,24 +1156,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
       <c r="F1" s="6"/>
       <c r="G1" s="21"/>
       <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="7" t="s">
         <v>26</v>
       </c>
@@ -1450,10 +1466,10 @@
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="28"/>
+      <c r="C15" s="25"/>
       <c r="D15" s="3">
         <v>8</v>
       </c>
@@ -1472,10 +1488,10 @@
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="3">
@@ -1496,10 +1512,10 @@
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="28"/>
+      <c r="C17" s="25"/>
       <c r="D17" s="3">
         <v>10</v>
       </c>
@@ -1518,10 +1534,10 @@
       <c r="A18" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="25"/>
       <c r="D18" s="3">
         <v>11</v>
       </c>
@@ -1540,10 +1556,10 @@
       <c r="A19" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="25"/>
       <c r="D19" s="3">
         <v>12</v>
       </c>
@@ -1562,10 +1578,10 @@
       <c r="A20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="28"/>
+      <c r="C20" s="25"/>
       <c r="D20" s="3">
         <v>13</v>
       </c>
@@ -1584,10 +1600,10 @@
       <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="25"/>
       <c r="D21" s="3">
         <v>14</v>
       </c>
@@ -1606,10 +1622,10 @@
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="3">
@@ -1630,10 +1646,10 @@
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D23" s="3">
@@ -1654,10 +1670,10 @@
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="3">
@@ -1678,10 +1694,10 @@
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="3">
@@ -1702,10 +1718,10 @@
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="3">
@@ -1726,10 +1742,10 @@
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="3">
@@ -1750,10 +1766,10 @@
       <c r="A28" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="3">
@@ -1774,10 +1790,10 @@
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="3">
@@ -1798,10 +1814,10 @@
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="25" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="3">
@@ -1822,10 +1838,10 @@
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="25" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="3">
@@ -1846,10 +1862,10 @@
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="25" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="3">
@@ -1870,10 +1886,10 @@
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="25" t="s">
         <v>67</v>
       </c>
       <c r="D33" s="3">
@@ -1894,10 +1910,10 @@
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D34" s="3">
@@ -1918,10 +1934,10 @@
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D35" s="3">
@@ -1942,7 +1958,7 @@
       <c r="A36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="26" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -1966,7 +1982,7 @@
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="26" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">

</xml_diff>

<commit_message>
2014 04 23 16:03
Criação das tabelas
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$40</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="71">
   <si>
     <t>Ação</t>
   </si>
@@ -262,6 +262,15 @@
   </si>
   <si>
     <t>T3 - Avalicação 2014-18</t>
+  </si>
+  <si>
+    <t>Tabela cidades</t>
+  </si>
+  <si>
+    <t>T3 - Avalicação 2014-3</t>
+  </si>
+  <si>
+    <t>Tabela  funcionarios</t>
   </si>
 </sst>
 </file>
@@ -585,7 +594,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -628,7 +637,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -671,7 +680,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -714,7 +723,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -762,7 +771,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -810,7 +819,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1136,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1264,22 +1273,22 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="D6" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="H6" s="5"/>
     </row>
@@ -1288,11 +1297,11 @@
         <v>39</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>10</v>
@@ -1310,23 +1319,24 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>66</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -1337,7 +1347,7 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>10</v>
@@ -1351,37 +1361,38 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" ht="21" customHeight="1">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>40</v>
+      <c r="B10" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="16">
-        <v>6</v>
-      </c>
-      <c r="E10" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3">
+        <v>5</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="16">
-        <v>6</v>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
+        <v>5</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>10</v>
@@ -1392,40 +1403,40 @@
       <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" ht="21" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="16">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="17" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3">
-        <v>7</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="16">
+        <v>6</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
@@ -1436,20 +1447,19 @@
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="21" customHeight="1">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="3">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="D14" s="16">
+        <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>9</v>
@@ -1460,18 +1470,17 @@
       <c r="G14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="25"/>
+      <c r="B15" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -1488,14 +1497,14 @@
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>9</v>
@@ -1508,16 +1517,16 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="20.25" customHeight="1">
+    <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>42</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -1526,23 +1535,25 @@
         <v>65</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="20.25" customHeight="1">
+    <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="D18" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>65</v>
@@ -1557,11 +1568,11 @@
         <v>44</v>
       </c>
       <c r="B19" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -1576,14 +1587,14 @@
     </row>
     <row r="20" spans="1:8" ht="20.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="25"/>
       <c r="D20" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
@@ -1598,14 +1609,14 @@
     </row>
     <row r="21" spans="1:8" ht="20.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
@@ -1620,19 +1631,17 @@
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>31</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="25"/>
       <c r="D22" s="3">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>65</v>
@@ -1644,19 +1653,17 @@
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="25" t="s">
-        <v>31</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C23" s="25"/>
       <c r="D23" s="3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>65</v>
@@ -1670,17 +1677,17 @@
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="27" t="s">
-        <v>53</v>
+      <c r="B24" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="C24" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>65</v>
@@ -1695,13 +1702,13 @@
         <v>8</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C25" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D25" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>9</v>
@@ -1719,13 +1726,13 @@
         <v>8</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="3">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>10</v>
@@ -1740,16 +1747,16 @@
     </row>
     <row r="27" spans="1:8" ht="20.25" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="3">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
@@ -1762,21 +1769,21 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="21" customHeight="1">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>65</v>
@@ -1786,21 +1793,21 @@
       </c>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="21" customHeight="1">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>65</v>
@@ -1815,16 +1822,16 @@
         <v>15</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D30" s="3">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>65</v>
@@ -1839,16 +1846,16 @@
         <v>15</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" s="3">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>65</v>
@@ -1863,13 +1870,13 @@
         <v>15</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D32" s="3">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>10</v>
@@ -1887,13 +1894,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>67</v>
+        <v>35</v>
       </c>
       <c r="D33" s="3">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>9</v>
@@ -1911,13 +1918,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D34" s="3">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>10</v>
@@ -1935,15 +1942,15 @@
         <v>15</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="D35" s="3">
-        <v>28</v>
-      </c>
-      <c r="E35" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -1952,20 +1959,20 @@
       <c r="G35" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H35" s="1"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="21" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>31</v>
       </c>
       <c r="D36" s="3">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>10</v>
@@ -1974,51 +1981,99 @@
         <v>65</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H36" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="21" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>28</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" ht="21" customHeight="1">
+      <c r="A38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="3">
+        <v>29</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" ht="21" customHeight="1">
+      <c r="A39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D39" s="3">
         <v>30</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G37" s="3" t="s">
+      <c r="F39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A38" s="11" t="s">
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A40" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B38" s="20">
-        <f>COUNTA(B4:B37)</f>
-        <v>34</v>
-      </c>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="14"/>
+      <c r="B40" s="20">
+        <f>COUNTA(B4:B39)</f>
+        <v>36</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G38"/>
+  <autoFilter ref="A3:G40"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 04 23 20:29
Conclusão da criação das tabelas
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$43</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="72">
   <si>
     <t>Ação</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Tabela  funcionarios</t>
+  </si>
+  <si>
+    <t>Tabela bonus</t>
   </si>
 </sst>
 </file>
@@ -594,7 +597,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -637,7 +640,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -680,7 +683,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -723,7 +726,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -771,7 +774,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -819,7 +822,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1145,16 +1148,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="57" style="17" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" style="17" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" style="19" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" style="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" style="16" customWidth="1"/>
@@ -1465,7 +1468,7 @@
         <v>9</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>66</v>
@@ -1510,7 +1513,7 @@
         <v>9</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>66</v>
@@ -1543,36 +1546,36 @@
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="25" t="s">
+      <c r="B18" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="20.25" customHeight="1">
+    <row r="19" spans="1:8" ht="21" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" s="27" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>71</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="3">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -1581,42 +1584,44 @@
         <v>65</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="20.25" customHeight="1">
+    <row r="20" spans="1:8" ht="21" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" s="25"/>
+        <v>8</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>31</v>
+      </c>
       <c r="D20" s="3">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="20.25" customHeight="1">
+    <row r="21" spans="1:8" ht="21" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>43</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="3">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
@@ -1631,14 +1636,14 @@
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>10</v>
@@ -1653,14 +1658,14 @@
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="3">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>10</v>
@@ -1675,19 +1680,17 @@
     </row>
     <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>31</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="25"/>
       <c r="D24" s="3">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>65</v>
@@ -1699,19 +1702,17 @@
     </row>
     <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>31</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C25" s="25"/>
       <c r="D25" s="3">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>65</v>
@@ -1723,16 +1724,14 @@
     </row>
     <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" s="25" t="s">
-        <v>31</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C26" s="25"/>
       <c r="D26" s="3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>10</v>
@@ -1749,14 +1748,14 @@
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="27" t="s">
-        <v>55</v>
+      <c r="B27" s="28" t="s">
+        <v>51</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
@@ -1774,16 +1773,16 @@
         <v>8</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D28" s="3">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F28" s="4" t="s">
         <v>65</v>
@@ -1795,19 +1794,19 @@
     </row>
     <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="3">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>65</v>
@@ -1817,18 +1816,18 @@
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="21" customHeight="1">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="3">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>9</v>
@@ -1841,18 +1840,18 @@
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="21" customHeight="1">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>10</v>
@@ -1865,21 +1864,21 @@
       </c>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="21" customHeight="1">
+    <row r="32" spans="1:8" ht="20.25" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D32" s="3">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>65</v>
@@ -1894,13 +1893,13 @@
         <v>15</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D33" s="3">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>9</v>
@@ -1918,13 +1917,13 @@
         <v>15</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D34" s="3">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>10</v>
@@ -1942,16 +1941,16 @@
         <v>15</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="D35" s="3">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>65</v>
@@ -1966,16 +1965,16 @@
         <v>15</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D36" s="3">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>65</v>
@@ -1990,16 +1989,16 @@
         <v>15</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D37" s="3">
-        <v>28</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>65</v>
@@ -2007,73 +2006,145 @@
       <c r="G37" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H37" s="1"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="21" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>35</v>
+        <v>15</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="D38" s="3">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>65</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="21" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="3">
+        <v>27</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="1:8" ht="21" customHeight="1">
+      <c r="A40" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" s="3">
+        <v>28</v>
+      </c>
+      <c r="E40" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" ht="21" customHeight="1">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="3">
+        <v>29</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" ht="21" customHeight="1">
+      <c r="A42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D42" s="3">
         <v>30</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="3" t="s">
+      <c r="F42" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A40" s="11" t="s">
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" s="18" customFormat="1" ht="26.25" customHeight="1">
+      <c r="A43" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="20">
-        <f>COUNTA(B4:B39)</f>
-        <v>36</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="14"/>
+      <c r="B43" s="20">
+        <f>COUNTA(B4:B42)</f>
+        <v>39</v>
+      </c>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G40"/>
+  <autoFilter ref="A3:G43"/>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>

<commit_message>
2014 04 26   14:05
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="73">
   <si>
     <t>Ação</t>
   </si>
@@ -274,12 +274,15 @@
   </si>
   <si>
     <t>Tabela bonus</t>
+  </si>
+  <si>
+    <t>Tabela venda_Itens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -860,6 +863,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 23"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="8848725" cy="15344775"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -938,6 +989,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -972,6 +1024,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1147,11 +1200,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1310,7 +1363,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>14</v>
@@ -1356,7 +1409,7 @@
         <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
@@ -1401,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>14</v>
@@ -1445,7 +1498,7 @@
         <v>10</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>14</v>
@@ -1489,7 +1542,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>14</v>
@@ -1501,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
2014 04 27   14:51
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
   <si>
     <t>Ação</t>
   </si>
@@ -123,9 +123,6 @@
     <t xml:space="preserve">Estrutura da atividade </t>
   </si>
   <si>
-    <t>Obs todas as tabélas e funções serão em aquivos individuais</t>
-  </si>
-  <si>
     <t xml:space="preserve">Todas as tabelas e funções </t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Tabela venda</t>
   </si>
   <si>
-    <t>Tabela venda_Intens</t>
-  </si>
-  <si>
     <t>Tabela Comissoes</t>
   </si>
   <si>
@@ -276,7 +270,10 @@
     <t>Tabela bonus</t>
   </si>
   <si>
-    <t>Tabela venda_Itens</t>
+    <t>Tabela vendas_itens</t>
+  </si>
+  <si>
+    <t>Obs.: Todas as tabelas e funções serão em aquivos individuais</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1201,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1222,7 +1219,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="15" customFormat="1" ht="15">
       <c r="A1" s="29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="30"/>
@@ -1234,13 +1231,13 @@
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1">
       <c r="A2" s="31" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
       <c r="D2" s="31"/>
       <c r="E2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="22">
         <v>41757</v>
@@ -1284,7 +1281,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -1308,7 +1305,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -1329,10 +1326,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3">
         <v>2</v>
@@ -1344,16 +1341,16 @@
         <v>18</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="21" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3">
@@ -1362,9 +1359,7 @@
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1375,10 +1370,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>4</v>
@@ -1396,10 +1391,10 @@
     </row>
     <row r="9" spans="1:8" ht="21" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3">
@@ -1408,9 +1403,7 @@
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F9" s="4"/>
       <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1421,10 +1414,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="3">
         <v>5</v>
@@ -1436,15 +1429,15 @@
         <v>18</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3">
@@ -1453,9 +1446,7 @@
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F11" s="4"/>
       <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1466,10 +1457,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="16">
         <v>6</v>
@@ -1481,15 +1472,15 @@
         <v>18</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" customHeight="1">
       <c r="A13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>40</v>
       </c>
       <c r="D13" s="16">
         <v>6</v>
@@ -1497,9 +1488,7 @@
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F13" s="4"/>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1509,10 +1498,10 @@
         <v>8</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="16">
         <v>7</v>
@@ -1524,15 +1513,15 @@
         <v>18</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3">
@@ -1541,9 +1530,7 @@
       <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="F15" s="4"/>
       <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1554,10 +1541,10 @@
         <v>8</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3">
         <v>8</v>
@@ -1569,16 +1556,16 @@
         <v>18</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="3">
@@ -1588,7 +1575,7 @@
         <v>10</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>14</v>
@@ -1600,10 +1587,10 @@
         <v>8</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="3">
         <v>8</v>
@@ -1615,16 +1602,16 @@
         <v>18</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="21" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="25"/>
       <c r="D19" s="3">
@@ -1634,7 +1621,7 @@
         <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>14</v>
@@ -1646,10 +1633,10 @@
         <v>8</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" s="3">
         <v>9</v>
@@ -1661,16 +1648,16 @@
         <v>18</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="21" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="25"/>
       <c r="D21" s="3">
@@ -1680,19 +1667,19 @@
         <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="27" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="C22" s="25"/>
       <c r="D22" s="3">
@@ -1702,19 +1689,19 @@
         <v>10</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="25"/>
       <c r="D23" s="3">
@@ -1724,19 +1711,19 @@
         <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="25"/>
       <c r="D24" s="3">
@@ -1746,19 +1733,19 @@
         <v>10</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="25"/>
       <c r="D25" s="3">
@@ -1768,19 +1755,19 @@
         <v>10</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="25"/>
       <c r="D26" s="3">
@@ -1790,10 +1777,10 @@
         <v>10</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H26" s="5"/>
     </row>
@@ -1802,10 +1789,10 @@
         <v>8</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D27" s="3">
         <v>15</v>
@@ -1814,10 +1801,10 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H27" s="5"/>
     </row>
@@ -1826,10 +1813,10 @@
         <v>8</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="3">
         <v>16</v>
@@ -1838,10 +1825,10 @@
         <v>9</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H28" s="5"/>
     </row>
@@ -1850,10 +1837,10 @@
         <v>8</v>
       </c>
       <c r="B29" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="3">
         <v>17</v>
@@ -1862,10 +1849,10 @@
         <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H29" s="5"/>
     </row>
@@ -1874,10 +1861,10 @@
         <v>8</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="3">
         <v>18</v>
@@ -1886,10 +1873,10 @@
         <v>9</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H30" s="5"/>
     </row>
@@ -1898,10 +1885,10 @@
         <v>8</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" s="3">
         <v>19</v>
@@ -1910,10 +1897,10 @@
         <v>10</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H31" s="5"/>
     </row>
@@ -1922,10 +1909,10 @@
         <v>15</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D32" s="3">
         <v>20</v>
@@ -1934,10 +1921,10 @@
         <v>9</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H32" s="5"/>
     </row>
@@ -1946,10 +1933,10 @@
         <v>15</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="3">
         <v>21</v>
@@ -1958,10 +1945,10 @@
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H33" s="5"/>
     </row>
@@ -1970,10 +1957,10 @@
         <v>15</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="3">
         <v>22</v>
@@ -1982,10 +1969,10 @@
         <v>10</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H34" s="5"/>
     </row>
@@ -1994,10 +1981,10 @@
         <v>15</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="3">
         <v>23</v>
@@ -2006,10 +1993,10 @@
         <v>10</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H35" s="5"/>
     </row>
@@ -2018,10 +2005,10 @@
         <v>15</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="3">
         <v>24</v>
@@ -2030,10 +2017,10 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H36" s="5"/>
     </row>
@@ -2042,10 +2029,10 @@
         <v>15</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" s="3">
         <v>25</v>
@@ -2054,10 +2041,10 @@
         <v>10</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H37" s="5"/>
     </row>
@@ -2066,10 +2053,10 @@
         <v>15</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D38" s="3">
         <v>26</v>
@@ -2078,10 +2065,10 @@
         <v>9</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H38" s="5"/>
     </row>
@@ -2090,10 +2077,10 @@
         <v>15</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D39" s="3">
         <v>27</v>
@@ -2102,10 +2089,10 @@
         <v>10</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H39" s="5"/>
     </row>
@@ -2114,10 +2101,10 @@
         <v>15</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D40" s="3">
         <v>28</v>
@@ -2126,10 +2113,10 @@
         <v>9</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -2138,10 +2125,10 @@
         <v>13</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="3">
         <v>29</v>
@@ -2150,7 +2137,7 @@
         <v>10</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G41" s="3" t="s">
         <v>14</v>
@@ -2165,7 +2152,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="3">
         <v>30</v>
@@ -2174,7 +2161,7 @@
         <v>9</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
2014 04 27 15:40
Criaão das View
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -282,7 +282,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -989,7 +989,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1024,7 +1023,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1200,11 +1198,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1814,7 +1812,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>66</v>
@@ -1838,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>66</v>
@@ -2126,7 +2124,7 @@
         <v>9</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
2014 04 27 15:18
Funções
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1202,7 +1202,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1884,7 +1884,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>66</v>

</xml_diff>

<commit_message>
2014 04 27 17:08
Conclusão das atividades da agenda
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="74">
   <si>
     <t>Ação</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>Tabela venda_Itens</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -1199,11 +1202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="F3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1275,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" hidden="1" customHeight="1">
+    <row r="4" spans="1:8" ht="25.5" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1299,7 +1301,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="5" spans="1:8" ht="21" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1323,7 +1325,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="6" spans="1:8" ht="21" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +1349,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="7" spans="1:8" ht="21" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1369,7 +1371,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="8" spans="1:8" ht="21" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1393,7 +1395,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="9" spans="1:8" ht="21" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1417,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="10" spans="1:8" ht="21" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="11" spans="1:8" ht="21" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1460,7 +1462,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="12" spans="1:8" ht="21" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1483,7 +1485,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="13" spans="1:8" ht="21" customHeight="1">
       <c r="A13" s="17" t="s">
         <v>39</v>
       </c>
@@ -1503,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="14" spans="1:8" ht="21" customHeight="1">
       <c r="A14" s="17" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1528,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="15" spans="1:8" ht="21" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1548,7 +1550,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="16" spans="1:8" ht="21" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -1572,7 +1574,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="17" spans="1:8" ht="21" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1594,7 +1596,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="18" spans="1:8" ht="21" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1618,7 +1620,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="19" spans="1:8" ht="21" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1640,7 +1642,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="20" spans="1:8" ht="21" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1664,7 +1666,7 @@
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="21" spans="1:8" ht="21" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -1686,7 +1688,7 @@
       </c>
       <c r="H21" s="5"/>
     </row>
-    <row r="22" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="22" spans="1:8" ht="20.25" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -1708,7 +1710,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="23" spans="1:8" ht="20.25" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -1730,7 +1732,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="24" spans="1:8" ht="20.25" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1752,7 +1754,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="25" spans="1:8" ht="20.25" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -1774,7 +1776,7 @@
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="26" spans="1:8" ht="20.25" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -1796,7 +1798,7 @@
       </c>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="27" spans="1:8" ht="20.25" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -1820,7 +1822,7 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="28" spans="1:8" ht="20.25" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -1844,7 +1846,7 @@
       </c>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="29" spans="1:8" ht="20.25" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -1868,7 +1870,7 @@
       </c>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="30" spans="1:8" ht="20.25" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -1892,7 +1894,7 @@
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="20.25" hidden="1" customHeight="1">
+    <row r="31" spans="1:8" ht="20.25" customHeight="1">
       <c r="A31" s="1" t="s">
         <v>8</v>
       </c>
@@ -1933,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>66</v>
@@ -1954,7 +1956,7 @@
         <v>21</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>65</v>
@@ -1964,7 +1966,7 @@
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="34" spans="1:8" ht="21" customHeight="1">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -1988,7 +1990,7 @@
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="35" spans="1:8" ht="21" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
@@ -2012,7 +2014,7 @@
       </c>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="36" spans="1:8" ht="21" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -2036,7 +2038,7 @@
       </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="37" spans="1:8" ht="21" customHeight="1">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -2077,14 +2079,14 @@
         <v>9</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H38" s="5"/>
     </row>
-    <row r="39" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="39" spans="1:8" ht="21" customHeight="1">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -2108,7 +2110,7 @@
       </c>
       <c r="H39" s="5"/>
     </row>
-    <row r="40" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="40" spans="1:8" ht="21" customHeight="1">
       <c r="A40" s="1" t="s">
         <v>15</v>
       </c>
@@ -2132,7 +2134,7 @@
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:8" ht="21" hidden="1" customHeight="1">
+    <row r="41" spans="1:8" ht="21" customHeight="1">
       <c r="A41" s="1" t="s">
         <v>13</v>
       </c>
@@ -2197,16 +2199,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A3:G43">
-    <filterColumn colId="4">
-      <filters blank="1">
-        <filter val="Neimar"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters blank="1">
-        <filter val="?"/>
-      </filters>
-    </filterColumn>
+    <filterColumn colId="4"/>
+    <filterColumn colId="5"/>
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
2014 04 27 19:04
Coreação da Agenda
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="74">
   <si>
     <t>Ação</t>
   </si>
@@ -274,12 +274,18 @@
   </si>
   <si>
     <t>Obs.: Todas as tabelas e funções serão em aquivos individuais</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -986,7 +992,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1021,7 +1026,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1197,11 +1201,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1290,7 +1294,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>11</v>
@@ -1314,7 +1318,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>11</v>
@@ -1338,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>64</v>
@@ -1359,7 +1363,9 @@
       <c r="E7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1403,7 +1409,9 @@
       <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1446,7 +1454,9 @@
       <c r="E11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
@@ -1488,7 +1498,9 @@
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="4"/>
+      <c r="F13" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1530,7 +1542,9 @@
       <c r="E15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="4"/>
+      <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1801,7 +1815,7 @@
         <v>9</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>64</v>
@@ -1825,7 +1839,7 @@
         <v>9</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>64</v>
@@ -1873,7 +1887,7 @@
         <v>9</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>64</v>
@@ -1921,7 +1935,7 @@
         <v>9</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>64</v>
@@ -1945,7 +1959,7 @@
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>64</v>
@@ -2017,7 +2031,7 @@
         <v>9</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G36" s="3" t="s">
         <v>64</v>
@@ -2065,7 +2079,7 @@
         <v>9</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>64</v>
@@ -2113,7 +2127,7 @@
         <v>9</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
2014 04 28 08:26
Correção de funções
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1703,7 +1703,7 @@
         <v>10</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>64</v>
@@ -1725,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>64</v>
@@ -1747,7 +1747,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>64</v>
@@ -1769,7 +1769,7 @@
         <v>10</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>64</v>
@@ -1863,7 +1863,7 @@
         <v>10</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>64</v>
@@ -2007,7 +2007,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>64</v>
@@ -2103,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>63</v>
+        <v>18</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
2014 04 28   09:21
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="210" yWindow="600" windowWidth="15480" windowHeight="8640"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$3:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -285,7 +285,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -992,6 +992,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1026,6 +1027,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -1201,11 +1203,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>

</xml_diff>

<commit_message>
2014 04 27 10:27
dd
</commit_message>
<xml_diff>
--- a/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
+++ b/BD2_2M/T3 - Avalicação 2014-1/Agenda de projeto.xlsx
@@ -1204,10 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="22.5" customHeight="1"/>
@@ -1279,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" customHeight="1">
+    <row r="4" spans="1:8" ht="25.5" hidden="1" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1304,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="21" customHeight="1">
+    <row r="5" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +1328,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="21" customHeight="1">
+    <row r="6" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -1351,7 +1352,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="21" customHeight="1">
+    <row r="7" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -1373,7 +1374,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="21" customHeight="1">
+    <row r="8" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1390,14 +1391,14 @@
         <v>9</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1">
+    <row r="9" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>38</v>
       </c>
@@ -1419,7 +1420,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1">
+    <row r="10" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1436,13 +1437,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1">
+    <row r="11" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1464,7 +1465,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1">
+    <row r="12" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>8</v>
       </c>
@@ -1481,13 +1482,13 @@
         <v>9</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1">
+    <row r="13" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A13" s="17" t="s">
         <v>38</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>73</v>
+        <v>18</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>14</v>
@@ -1598,7 +1599,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1">
+    <row r="18" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -1615,14 +1616,14 @@
         <v>9</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="21" customHeight="1">
+    <row r="19" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
@@ -1637,14 +1638,14 @@
         <v>10</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="21" customHeight="1">
+    <row r="20" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1661,14 +1662,14 @@
         <v>9</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>64</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="21" customHeight="1">
+    <row r="21" spans="1:8" ht="21" hidden="1" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -1683,7 +1684,7 @@
         <v>10</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>64</v>
@@ -2200,7 +2201,15 @@
       <c r="H43" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G43"/>
+  <autoFilter ref="A3:G43">
+    <filterColumn colId="5">
+      <filters blank="1">
+        <filter val="!"/>
+        <filter val="*"/>
+        <filter val="?"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:D2"/>

</xml_diff>